<commit_message>
Updating Old File for core commit ea5b4bdc2033b934bc3b52118f1a3e5ca9f83838
</commit_message>
<xml_diff>
--- a/help/implementation/implementation-basics/assets/aa_en_BRD_SDR_template.xlsx
+++ b/help/implementation/implementation-basics/assets/aa_en_BRD_SDR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelehajala/Documents/GitHub/analytics-learn.en/help/implementation/implementation-basics/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0310E7D-96A6-EE41-B893-AE1B4A0894DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7E4642-3DCD-C64E-B45E-CF52611F785A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40940" yWindow="500" windowWidth="38400" windowHeight="19700" tabRatio="795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41020" yWindow="500" windowWidth="33540" windowHeight="17560" tabRatio="795" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="25" r:id="rId1"/>
@@ -11121,7 +11121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63318AAA-537C-414B-98C7-3448FFDA634A}">
   <dimension ref="A1:DX36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15828,7 +15828,7 @@
   <dimension ref="A1:P112"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight"/>
@@ -17998,10 +17998,10 @@
   <dimension ref="A1:S310"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F243" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26814,7 +26814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A5F1FE-3511-4C81-B0A0-0369494198BC}">
   <dimension ref="A1:O260"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -47677,9 +47677,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47821,26 +47824,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC145E80-3530-4461-96D8-8445D2DA91FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56E71D42-D722-48FC-AFB6-6742E952DC21}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="00ed0f5a-bba9-4357-a622-3ee042b985a0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -47864,9 +47856,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56E71D42-D722-48FC-AFB6-6742E952DC21}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC145E80-3530-4461-96D8-8445D2DA91FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="00ed0f5a-bba9-4357-a622-3ee042b985a0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>